<commit_message>
GCB cement carbonation fix
</commit_message>
<xml_diff>
--- a/results/ghg_emissions_co2e_2024.xlsx
+++ b/results/ghg_emissions_co2e_2024.xlsx
@@ -4751,7 +4751,7 @@
         <v>7.77893111111112</v>
       </c>
       <c r="F211" t="n">
-        <v>8.86110667023945</v>
+        <v>8.81511879903416</v>
       </c>
     </row>
     <row r="212">
@@ -4771,7 +4771,7 @@
         <v>6.83614555555554</v>
       </c>
       <c r="F212" t="n">
-        <v>9.39325277183355</v>
+        <v>9.34308524994097</v>
       </c>
     </row>
     <row r="213">
@@ -4791,7 +4791,7 @@
         <v>6.55410555555554</v>
       </c>
       <c r="F213" t="n">
-        <v>9.42123422086363</v>
+        <v>9.3678927496124</v>
       </c>
     </row>
     <row r="214">
@@ -4811,7 +4811,7 @@
         <v>6.07844111111112</v>
       </c>
       <c r="F214" t="n">
-        <v>9.75364952215122</v>
+        <v>9.69615667814099</v>
       </c>
     </row>
     <row r="215">
@@ -4831,7 +4831,7 @@
         <v>5.88154111111112</v>
       </c>
       <c r="F215" t="n">
-        <v>10.2735188654145</v>
+        <v>10.2124579227845</v>
       </c>
     </row>
     <row r="216">
@@ -4851,7 +4851,7 @@
         <v>5.73926222222221</v>
       </c>
       <c r="F216" t="n">
-        <v>10.8314954888097</v>
+        <v>10.7646888772226</v>
       </c>
     </row>
     <row r="217">
@@ -4871,7 +4871,7 @@
         <v>5.20934333333333</v>
       </c>
       <c r="F217" t="n">
-        <v>11.3179204851679</v>
+        <v>11.2474010247099</v>
       </c>
     </row>
     <row r="218">
@@ -4891,7 +4891,7 @@
         <v>5.03820777777779</v>
       </c>
       <c r="F218" t="n">
-        <v>11.8703414584522</v>
+        <v>11.7946512533543</v>
       </c>
     </row>
     <row r="219">
@@ -4911,7 +4911,7 @@
         <v>5.17441222222221</v>
       </c>
       <c r="F219" t="n">
-        <v>12.2452341052205</v>
+        <v>12.1658266145556</v>
       </c>
     </row>
     <row r="220">
@@ -4931,7 +4931,7 @@
         <v>5.23615888888888</v>
       </c>
       <c r="F220" t="n">
-        <v>12.9137275294203</v>
+        <v>12.8286255001192</v>
       </c>
     </row>
     <row r="221">
@@ -4951,7 +4951,7 @@
         <v>4.91510555555554</v>
       </c>
       <c r="F221" t="n">
-        <v>13.7708545683368</v>
+        <v>13.680537267521</v>
       </c>
     </row>
     <row r="222">
@@ -4971,7 +4971,7 @@
         <v>5.11790888888888</v>
       </c>
       <c r="F222" t="n">
-        <v>14.9089992772999</v>
+        <v>14.8131918088562</v>
       </c>
     </row>
     <row r="223">
@@ -4991,7 +4991,7 @@
         <v>4.82282777777779</v>
       </c>
       <c r="F223" t="n">
-        <v>15.5140686710042</v>
+        <v>15.4128693208505</v>
       </c>
     </row>
     <row r="224">
@@ -5011,7 +5011,7 @@
         <v>4.82573666666667</v>
       </c>
       <c r="F224" t="n">
-        <v>16.2352471608668</v>
+        <v>16.1249902711566</v>
       </c>
     </row>
     <row r="225">
@@ -5031,7 +5031,7 @@
         <v>4.69871111111112</v>
       </c>
       <c r="F225" t="n">
-        <v>17.0959340035456</v>
+        <v>16.9779788472047</v>
       </c>
     </row>
     <row r="226">
@@ -5051,7 +5051,7 @@
         <v>4.56748111111112</v>
       </c>
       <c r="F226" t="n">
-        <v>17.0217615898472</v>
+        <v>16.9010329704924</v>
       </c>
     </row>
     <row r="227">
@@ -5071,7 +5071,7 @@
         <v>4.61616222222221</v>
       </c>
       <c r="F227" t="n">
-        <v>17.0623883610057</v>
+        <v>16.9392086052925</v>
       </c>
     </row>
     <row r="228">
@@ -5091,7 +5091,7 @@
         <v>4.59416222222221</v>
       </c>
       <c r="F228" t="n">
-        <v>17.998334699753</v>
+        <v>17.8680891333005</v>
       </c>
     </row>
     <row r="229">
@@ -5111,7 +5111,7 @@
         <v>4.59456555555554</v>
       </c>
       <c r="F229" t="n">
-        <v>18.5081120165744</v>
+        <v>18.3691936178106</v>
       </c>
     </row>
     <row r="230">
@@ -5131,7 +5131,7 @@
         <v>4.45968111111112</v>
       </c>
       <c r="F230" t="n">
-        <v>19.0778298086923</v>
+        <v>18.9293079380494</v>
       </c>
     </row>
     <row r="231">
@@ -5151,7 +5151,7 @@
         <v>4.23270222222221</v>
       </c>
       <c r="F231" t="n">
-        <v>19.6172693155098</v>
+        <v>19.463412918274</v>
       </c>
     </row>
     <row r="232">
@@ -5171,7 +5171,7 @@
         <v>4.40971666666667</v>
       </c>
       <c r="F232" t="n">
-        <v>19.49661997436</v>
+        <v>19.3382592597337</v>
       </c>
     </row>
     <row r="233">
@@ -5191,7 +5191,7 @@
         <v>4.65830444444446</v>
       </c>
       <c r="F233" t="n">
-        <v>19.0307895360311</v>
+        <v>18.8692963551612</v>
       </c>
     </row>
     <row r="234">
@@ -5211,7 +5211,7 @@
         <v>4.68006</v>
       </c>
       <c r="F234" t="n">
-        <v>18.8791034478427</v>
+        <v>18.7146881145726</v>
       </c>
     </row>
     <row r="235">
@@ -5231,7 +5231,7 @@
         <v>5.16343666666667</v>
       </c>
       <c r="F235" t="n">
-        <v>18.9997192912982</v>
+        <v>18.8299392297625</v>
       </c>
     </row>
     <row r="236">
@@ -5251,7 +5251,7 @@
         <v>5.97128888888888</v>
       </c>
       <c r="F236" t="n">
-        <v>19.6560239450458</v>
+        <v>19.4810879898412</v>
       </c>
     </row>
     <row r="237">
@@ -5271,7 +5271,7 @@
         <v>5.50831111111112</v>
       </c>
       <c r="F237" t="n">
-        <v>20.3199086356009</v>
+        <v>20.140086361496</v>
       </c>
     </row>
     <row r="238">
@@ -5291,7 +5291,7 @@
         <v>5.69696111111112</v>
       </c>
       <c r="F238" t="n">
-        <v>20.622511031547</v>
+        <v>20.4341660472957</v>
       </c>
     </row>
     <row r="239">
@@ -5311,7 +5311,7 @@
         <v>5.51857777777779</v>
       </c>
       <c r="F239" t="n">
-        <v>21.2612456481135</v>
+        <v>21.0641965048392</v>
       </c>
     </row>
     <row r="240">
@@ -5331,7 +5331,7 @@
         <v>5.30255</v>
       </c>
       <c r="F240" t="n">
-        <v>22.0934528378386</v>
+        <v>21.8848057811506</v>
       </c>
     </row>
     <row r="241">
@@ -5351,7 +5351,7 @@
         <v>5.24466555555554</v>
       </c>
       <c r="F241" t="n">
-        <v>22.3952569616586</v>
+        <v>22.1871546787502</v>
       </c>
     </row>
     <row r="242">
@@ -5371,7 +5371,7 @@
         <v>5.17066</v>
       </c>
       <c r="F242" t="n">
-        <v>22.7692597354242</v>
+        <v>22.5634645176629</v>
       </c>
     </row>
     <row r="243">
@@ -5391,7 +5391,7 @@
         <v>4.95013444444446</v>
       </c>
       <c r="F243" t="n">
-        <v>23.2463815873576</v>
+        <v>23.0281143426953</v>
       </c>
     </row>
     <row r="244">
@@ -5411,7 +5411,7 @@
         <v>5.22690666666667</v>
       </c>
       <c r="F244" t="n">
-        <v>22.5836234207144</v>
+        <v>22.3625406807364</v>
       </c>
     </row>
     <row r="245">
@@ -5431,7 +5431,7 @@
         <v>5.13279555555554</v>
       </c>
       <c r="F245" t="n">
-        <v>22.8149429858478</v>
+        <v>22.5788003906778</v>
       </c>
     </row>
     <row r="246">
@@ -5451,7 +5451,7 @@
         <v>5.78063444444446</v>
       </c>
       <c r="F246" t="n">
-        <v>23.0515398353275</v>
+        <v>22.8026647582914</v>
       </c>
     </row>
     <row r="247">
@@ -5471,7 +5471,7 @@
         <v>5.64358666666667</v>
       </c>
       <c r="F247" t="n">
-        <v>23.541613095877</v>
+        <v>23.2794145115452</v>
       </c>
     </row>
     <row r="248">
@@ -5491,7 +5491,7 @@
         <v>6.00167333333333</v>
       </c>
       <c r="F248" t="n">
-        <v>24.2678121915624</v>
+        <v>23.9956955875247</v>
       </c>
     </row>
     <row r="249">
@@ -5511,7 +5511,7 @@
         <v>7.48644111111112</v>
       </c>
       <c r="F249" t="n">
-        <v>24.413705934332</v>
+        <v>24.1314365237098</v>
       </c>
     </row>
     <row r="250">
@@ -5531,7 +5531,7 @@
         <v>6.16961888888888</v>
       </c>
       <c r="F250" t="n">
-        <v>24.3486537711564</v>
+        <v>24.0635808416072</v>
       </c>
     </row>
     <row r="251">
@@ -5551,7 +5551,7 @@
         <v>6.00837111111112</v>
       </c>
       <c r="F251" t="n">
-        <v>24.8515684964607</v>
+        <v>24.5563558977527</v>
       </c>
     </row>
     <row r="252">
@@ -5571,7 +5571,7 @@
         <v>5.37957444444446</v>
       </c>
       <c r="F252" t="n">
-        <v>25.5198476641384</v>
+        <v>25.2135455590157</v>
       </c>
     </row>
     <row r="253">
@@ -5591,7 +5591,7 @@
         <v>5.03983333333333</v>
       </c>
       <c r="F253" t="n">
-        <v>25.6936166097304</v>
+        <v>25.3778821395335</v>
       </c>
     </row>
     <row r="254">
@@ -5611,7 +5611,7 @@
         <v>5.38909555555554</v>
       </c>
       <c r="F254" t="n">
-        <v>26.2673930172504</v>
+        <v>25.9354754639054</v>
       </c>
     </row>
     <row r="255">
@@ -5631,7 +5631,7 @@
         <v>5.83778555555554</v>
       </c>
       <c r="F255" t="n">
-        <v>27.6687720478414</v>
+        <v>27.3120969910027</v>
       </c>
     </row>
     <row r="256">
@@ -5651,7 +5651,7 @@
         <v>5.39773666666667</v>
       </c>
       <c r="F256" t="n">
-        <v>28.6410224441935</v>
+        <v>28.2594511675065</v>
       </c>
     </row>
     <row r="257">
@@ -5671,7 +5671,7 @@
         <v>4.89546444444446</v>
       </c>
       <c r="F257" t="n">
-        <v>29.6136400579236</v>
+        <v>29.2060498412086</v>
       </c>
     </row>
     <row r="258">
@@ -5691,7 +5691,7 @@
         <v>5.23851777777779</v>
       </c>
       <c r="F258" t="n">
-        <v>30.6280421147188</v>
+        <v>30.1843076977275</v>
       </c>
     </row>
     <row r="259">
@@ -5711,7 +5711,7 @@
         <v>4.55935333333333</v>
       </c>
       <c r="F259" t="n">
-        <v>31.5226595855864</v>
+        <v>31.0446436637643</v>
       </c>
     </row>
     <row r="260">
@@ -5731,7 +5731,7 @@
         <v>4.74423888888888</v>
       </c>
       <c r="F260" t="n">
-        <v>32.0652226871211</v>
+        <v>31.5714666004947</v>
       </c>
     </row>
     <row r="261">
@@ -5751,7 +5751,7 @@
         <v>5.23996</v>
       </c>
       <c r="F261" t="n">
-        <v>31.5161874394197</v>
+        <v>30.9973086908139</v>
       </c>
     </row>
     <row r="262">
@@ -5771,7 +5771,7 @@
         <v>5.18128111111112</v>
       </c>
       <c r="F262" t="n">
-        <v>33.3305683950991</v>
+        <v>32.7795448574245</v>
       </c>
     </row>
     <row r="263">
@@ -5791,7 +5791,7 @@
         <v>5.22179777777779</v>
       </c>
       <c r="F263" t="n">
-        <v>34.4615334801566</v>
+        <v>33.8648968341852</v>
       </c>
     </row>
     <row r="264">
@@ -5811,7 +5811,7 @@
         <v>5.34908</v>
       </c>
       <c r="F264" t="n">
-        <v>34.9608794652061</v>
+        <v>34.3403339697267</v>
       </c>
     </row>
     <row r="265">
@@ -5831,7 +5831,7 @@
         <v>4.86231777777779</v>
       </c>
       <c r="F265" t="n">
-        <v>35.2581093692935</v>
+        <v>34.608268884678</v>
       </c>
     </row>
     <row r="266">
@@ -5851,7 +5851,7 @@
         <v>5.21808222222221</v>
       </c>
       <c r="F266" t="n">
-        <v>35.4920072074535</v>
+        <v>34.8139228007151</v>
       </c>
     </row>
     <row r="267">
@@ -5871,7 +5871,7 @@
         <v>5.63435888888888</v>
       </c>
       <c r="F267" t="n">
-        <v>35.4890249614064</v>
+        <v>34.8072489147343</v>
       </c>
     </row>
     <row r="268">
@@ -5891,7 +5891,7 @@
         <v>4.60233888888888</v>
       </c>
       <c r="F268" t="n">
-        <v>35.4858335294738</v>
+        <v>34.7964857013939</v>
       </c>
     </row>
     <row r="269">
@@ -5911,7 +5911,7 @@
         <v>4.56831222222221</v>
       </c>
       <c r="F269" t="n">
-        <v>36.0516707578901</v>
+        <v>35.3474044986642</v>
       </c>
     </row>
     <row r="270">
@@ -5931,7 +5931,7 @@
         <v>4.28826444444446</v>
       </c>
       <c r="F270" t="n">
-        <v>36.7937041658923</v>
+        <v>36.0669868814637</v>
       </c>
     </row>
     <row r="271">
@@ -5951,7 +5951,7 @@
         <v>4.60086</v>
       </c>
       <c r="F271" t="n">
-        <v>37.0670612508218</v>
+        <v>36.3279228652471</v>
       </c>
     </row>
     <row r="272">
@@ -5971,7 +5971,7 @@
         <v>4.29831111111112</v>
       </c>
       <c r="F272" t="n">
-        <v>35.0332176239559</v>
+        <v>34.2747392419927</v>
       </c>
     </row>
     <row r="273">
@@ -5991,7 +5991,7 @@
         <v>4.32472333333333</v>
       </c>
       <c r="F273" t="n">
-        <v>36.8433375946504</v>
+        <v>36.0496417380356</v>
       </c>
     </row>
     <row r="274">
@@ -6011,7 +6011,7 @@
         <v>4.31308777777779</v>
       </c>
       <c r="F274" t="n">
-        <v>37.1768224213925</v>
+        <v>36.3794521675663</v>
       </c>
     </row>
     <row r="275">
@@ -6073,7 +6073,7 @@
         <v>26</v>
       </c>
       <c r="E2" t="n">
-        <v>8.86110667023945</v>
+        <v>8.81511879903416</v>
       </c>
     </row>
     <row r="3">
@@ -6090,7 +6090,7 @@
         <v>27</v>
       </c>
       <c r="E3" t="n">
-        <v>9.39325277183355</v>
+        <v>9.34308524994097</v>
       </c>
     </row>
     <row r="4">
@@ -6107,7 +6107,7 @@
         <v>28</v>
       </c>
       <c r="E4" t="n">
-        <v>9.42123422086363</v>
+        <v>9.3678927496124</v>
       </c>
     </row>
     <row r="5">
@@ -6124,7 +6124,7 @@
         <v>29</v>
       </c>
       <c r="E5" t="n">
-        <v>9.75364952215122</v>
+        <v>9.69615667814099</v>
       </c>
     </row>
     <row r="6">
@@ -6141,7 +6141,7 @@
         <v>30</v>
       </c>
       <c r="E6" t="n">
-        <v>10.2735188654145</v>
+        <v>10.2124579227845</v>
       </c>
     </row>
     <row r="7">
@@ -6158,7 +6158,7 @@
         <v>31</v>
       </c>
       <c r="E7" t="n">
-        <v>10.8314954888097</v>
+        <v>10.7646888772226</v>
       </c>
     </row>
     <row r="8">
@@ -6175,7 +6175,7 @@
         <v>32</v>
       </c>
       <c r="E8" t="n">
-        <v>11.3179204851679</v>
+        <v>11.2474010247099</v>
       </c>
     </row>
     <row r="9">
@@ -6192,7 +6192,7 @@
         <v>33</v>
       </c>
       <c r="E9" t="n">
-        <v>11.8703414584522</v>
+        <v>11.7946512533543</v>
       </c>
     </row>
     <row r="10">
@@ -6209,7 +6209,7 @@
         <v>34</v>
       </c>
       <c r="E10" t="n">
-        <v>12.2452341052205</v>
+        <v>12.1658266145556</v>
       </c>
     </row>
     <row r="11">
@@ -6226,7 +6226,7 @@
         <v>35</v>
       </c>
       <c r="E11" t="n">
-        <v>12.9137275294203</v>
+        <v>12.8286255001192</v>
       </c>
     </row>
     <row r="12">
@@ -6243,7 +6243,7 @@
         <v>36</v>
       </c>
       <c r="E12" t="n">
-        <v>13.7708545683368</v>
+        <v>13.680537267521</v>
       </c>
     </row>
     <row r="13">
@@ -6260,7 +6260,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="n">
-        <v>14.9089992772999</v>
+        <v>14.8131918088562</v>
       </c>
     </row>
     <row r="14">
@@ -6277,7 +6277,7 @@
         <v>38</v>
       </c>
       <c r="E14" t="n">
-        <v>15.5140686710042</v>
+        <v>15.4128693208505</v>
       </c>
     </row>
     <row r="15">
@@ -6294,7 +6294,7 @@
         <v>39</v>
       </c>
       <c r="E15" t="n">
-        <v>16.2352471608668</v>
+        <v>16.1249902711566</v>
       </c>
     </row>
     <row r="16">
@@ -6311,7 +6311,7 @@
         <v>40</v>
       </c>
       <c r="E16" t="n">
-        <v>17.0959340035456</v>
+        <v>16.9779788472047</v>
       </c>
     </row>
     <row r="17">
@@ -6328,7 +6328,7 @@
         <v>41</v>
       </c>
       <c r="E17" t="n">
-        <v>17.0217615898472</v>
+        <v>16.9010329704924</v>
       </c>
     </row>
     <row r="18">
@@ -6345,7 +6345,7 @@
         <v>42</v>
       </c>
       <c r="E18" t="n">
-        <v>17.0623883610057</v>
+        <v>16.9392086052925</v>
       </c>
     </row>
     <row r="19">
@@ -6362,7 +6362,7 @@
         <v>43</v>
       </c>
       <c r="E19" t="n">
-        <v>17.998334699753</v>
+        <v>17.8680891333005</v>
       </c>
     </row>
     <row r="20">
@@ -6379,7 +6379,7 @@
         <v>44</v>
       </c>
       <c r="E20" t="n">
-        <v>18.5081120165744</v>
+        <v>18.3691936178106</v>
       </c>
     </row>
     <row r="21">
@@ -6396,7 +6396,7 @@
         <v>45</v>
       </c>
       <c r="E21" t="n">
-        <v>19.0778298086923</v>
+        <v>18.9293079380494</v>
       </c>
     </row>
     <row r="22">
@@ -6413,7 +6413,7 @@
         <v>46</v>
       </c>
       <c r="E22" t="n">
-        <v>19.6172693155098</v>
+        <v>19.463412918274</v>
       </c>
     </row>
     <row r="23">
@@ -6430,7 +6430,7 @@
         <v>47</v>
       </c>
       <c r="E23" t="n">
-        <v>19.49661997436</v>
+        <v>19.3382592597337</v>
       </c>
     </row>
     <row r="24">
@@ -6447,7 +6447,7 @@
         <v>48</v>
       </c>
       <c r="E24" t="n">
-        <v>19.0307895360311</v>
+        <v>18.8692963551612</v>
       </c>
     </row>
     <row r="25">
@@ -6464,7 +6464,7 @@
         <v>49</v>
       </c>
       <c r="E25" t="n">
-        <v>18.8791034478427</v>
+        <v>18.7146881145726</v>
       </c>
     </row>
     <row r="26">
@@ -6481,7 +6481,7 @@
         <v>50</v>
       </c>
       <c r="E26" t="n">
-        <v>18.9997192912982</v>
+        <v>18.8299392297625</v>
       </c>
     </row>
     <row r="27">
@@ -6498,7 +6498,7 @@
         <v>51</v>
       </c>
       <c r="E27" t="n">
-        <v>19.6560239450458</v>
+        <v>19.4810879898412</v>
       </c>
     </row>
     <row r="28">
@@ -6515,7 +6515,7 @@
         <v>52</v>
       </c>
       <c r="E28" t="n">
-        <v>20.3199086356009</v>
+        <v>20.140086361496</v>
       </c>
     </row>
     <row r="29">
@@ -6532,7 +6532,7 @@
         <v>53</v>
       </c>
       <c r="E29" t="n">
-        <v>20.622511031547</v>
+        <v>20.4341660472957</v>
       </c>
     </row>
     <row r="30">
@@ -6549,7 +6549,7 @@
         <v>54</v>
       </c>
       <c r="E30" t="n">
-        <v>21.2612456481135</v>
+        <v>21.0641965048392</v>
       </c>
     </row>
     <row r="31">
@@ -6566,7 +6566,7 @@
         <v>55</v>
       </c>
       <c r="E31" t="n">
-        <v>22.0934528378386</v>
+        <v>21.8848057811506</v>
       </c>
     </row>
     <row r="32">
@@ -6583,7 +6583,7 @@
         <v>56</v>
       </c>
       <c r="E32" t="n">
-        <v>22.3952569616586</v>
+        <v>22.1871546787502</v>
       </c>
     </row>
     <row r="33">
@@ -6600,7 +6600,7 @@
         <v>57</v>
       </c>
       <c r="E33" t="n">
-        <v>22.7692597354242</v>
+        <v>22.5634645176629</v>
       </c>
     </row>
     <row r="34">
@@ -6617,7 +6617,7 @@
         <v>58</v>
       </c>
       <c r="E34" t="n">
-        <v>23.2463815873576</v>
+        <v>23.0281143426953</v>
       </c>
     </row>
     <row r="35">
@@ -6634,7 +6634,7 @@
         <v>59</v>
       </c>
       <c r="E35" t="n">
-        <v>22.5836234207144</v>
+        <v>22.3625406807364</v>
       </c>
     </row>
     <row r="36">
@@ -6651,7 +6651,7 @@
         <v>60</v>
       </c>
       <c r="E36" t="n">
-        <v>22.8149429858478</v>
+        <v>22.5788003906778</v>
       </c>
     </row>
     <row r="37">
@@ -6668,7 +6668,7 @@
         <v>61</v>
       </c>
       <c r="E37" t="n">
-        <v>23.0515398353275</v>
+        <v>22.8026647582914</v>
       </c>
     </row>
     <row r="38">
@@ -6685,7 +6685,7 @@
         <v>62</v>
       </c>
       <c r="E38" t="n">
-        <v>23.541613095877</v>
+        <v>23.2794145115452</v>
       </c>
     </row>
     <row r="39">
@@ -6702,7 +6702,7 @@
         <v>63</v>
       </c>
       <c r="E39" t="n">
-        <v>24.2678121915624</v>
+        <v>23.9956955875247</v>
       </c>
     </row>
     <row r="40">
@@ -6719,7 +6719,7 @@
         <v>64</v>
       </c>
       <c r="E40" t="n">
-        <v>24.413705934332</v>
+        <v>24.1314365237098</v>
       </c>
     </row>
     <row r="41">
@@ -6736,7 +6736,7 @@
         <v>65</v>
       </c>
       <c r="E41" t="n">
-        <v>24.3486537711564</v>
+        <v>24.0635808416072</v>
       </c>
     </row>
     <row r="42">
@@ -6753,7 +6753,7 @@
         <v>66</v>
       </c>
       <c r="E42" t="n">
-        <v>24.8515684964607</v>
+        <v>24.5563558977527</v>
       </c>
     </row>
     <row r="43">
@@ -6770,7 +6770,7 @@
         <v>67</v>
       </c>
       <c r="E43" t="n">
-        <v>25.5198476641384</v>
+        <v>25.2135455590157</v>
       </c>
     </row>
     <row r="44">
@@ -6787,7 +6787,7 @@
         <v>68</v>
       </c>
       <c r="E44" t="n">
-        <v>25.6936166097304</v>
+        <v>25.3778821395335</v>
       </c>
     </row>
     <row r="45">
@@ -6804,7 +6804,7 @@
         <v>69</v>
       </c>
       <c r="E45" t="n">
-        <v>26.2673930172504</v>
+        <v>25.9354754639054</v>
       </c>
     </row>
     <row r="46">
@@ -6821,7 +6821,7 @@
         <v>70</v>
       </c>
       <c r="E46" t="n">
-        <v>27.6687720478414</v>
+        <v>27.3120969910027</v>
       </c>
     </row>
     <row r="47">
@@ -6838,7 +6838,7 @@
         <v>71</v>
       </c>
       <c r="E47" t="n">
-        <v>28.6410224441935</v>
+        <v>28.2594511675065</v>
       </c>
     </row>
     <row r="48">
@@ -6855,7 +6855,7 @@
         <v>72</v>
       </c>
       <c r="E48" t="n">
-        <v>29.6136400579236</v>
+        <v>29.2060498412086</v>
       </c>
     </row>
     <row r="49">
@@ -6872,7 +6872,7 @@
         <v>73</v>
       </c>
       <c r="E49" t="n">
-        <v>30.6280421147188</v>
+        <v>30.1843076977275</v>
       </c>
     </row>
     <row r="50">
@@ -6889,7 +6889,7 @@
         <v>74</v>
       </c>
       <c r="E50" t="n">
-        <v>31.5226595855864</v>
+        <v>31.0446436637643</v>
       </c>
     </row>
     <row r="51">
@@ -6906,7 +6906,7 @@
         <v>75</v>
       </c>
       <c r="E51" t="n">
-        <v>32.0652226871211</v>
+        <v>31.5714666004947</v>
       </c>
     </row>
     <row r="52">
@@ -6923,7 +6923,7 @@
         <v>76</v>
       </c>
       <c r="E52" t="n">
-        <v>31.5161874394197</v>
+        <v>30.9973086908139</v>
       </c>
     </row>
     <row r="53">
@@ -6940,7 +6940,7 @@
         <v>77</v>
       </c>
       <c r="E53" t="n">
-        <v>33.3305683950991</v>
+        <v>32.7795448574245</v>
       </c>
     </row>
     <row r="54">
@@ -6957,7 +6957,7 @@
         <v>78</v>
       </c>
       <c r="E54" t="n">
-        <v>34.4615334801566</v>
+        <v>33.8648968341852</v>
       </c>
     </row>
     <row r="55">
@@ -6974,7 +6974,7 @@
         <v>79</v>
       </c>
       <c r="E55" t="n">
-        <v>34.9608794652061</v>
+        <v>34.3403339697267</v>
       </c>
     </row>
     <row r="56">
@@ -6991,7 +6991,7 @@
         <v>80</v>
       </c>
       <c r="E56" t="n">
-        <v>35.2581093692935</v>
+        <v>34.608268884678</v>
       </c>
     </row>
     <row r="57">
@@ -7008,7 +7008,7 @@
         <v>81</v>
       </c>
       <c r="E57" t="n">
-        <v>35.4920072074535</v>
+        <v>34.8139228007151</v>
       </c>
     </row>
     <row r="58">
@@ -7025,7 +7025,7 @@
         <v>82</v>
       </c>
       <c r="E58" t="n">
-        <v>35.4890249614064</v>
+        <v>34.8072489147343</v>
       </c>
     </row>
     <row r="59">
@@ -7042,7 +7042,7 @@
         <v>83</v>
       </c>
       <c r="E59" t="n">
-        <v>35.4858335294738</v>
+        <v>34.7964857013939</v>
       </c>
     </row>
     <row r="60">
@@ -7059,7 +7059,7 @@
         <v>84</v>
       </c>
       <c r="E60" t="n">
-        <v>36.0516707578901</v>
+        <v>35.3474044986642</v>
       </c>
     </row>
     <row r="61">
@@ -7076,7 +7076,7 @@
         <v>85</v>
       </c>
       <c r="E61" t="n">
-        <v>36.7937041658923</v>
+        <v>36.0669868814637</v>
       </c>
     </row>
     <row r="62">
@@ -7093,7 +7093,7 @@
         <v>86</v>
       </c>
       <c r="E62" t="n">
-        <v>37.0670612508218</v>
+        <v>36.3279228652471</v>
       </c>
     </row>
     <row r="63">
@@ -7110,7 +7110,7 @@
         <v>87</v>
       </c>
       <c r="E63" t="n">
-        <v>35.0332176239559</v>
+        <v>34.2747392419927</v>
       </c>
     </row>
     <row r="64">
@@ -7127,7 +7127,7 @@
         <v>88</v>
       </c>
       <c r="E64" t="n">
-        <v>36.8433375946504</v>
+        <v>36.0496417380356</v>
       </c>
     </row>
     <row r="65">
@@ -7144,7 +7144,7 @@
         <v>89</v>
       </c>
       <c r="E65" t="n">
-        <v>37.1768224213925</v>
+        <v>36.3794521675663</v>
       </c>
     </row>
     <row r="66">

</xml_diff>